<commit_message>
got fixing data scrape to work
</commit_message>
<xml_diff>
--- a/static/data/top2017_clean.xlsx
+++ b/static/data/top2017_clean.xlsx
@@ -1035,7 +1035,11 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>55n9yjI6qqXh5F2mYvUc2y</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>I Don’t Wanna Live Forever (Fifty Shades Darker)</t>

</xml_diff>

<commit_message>
added popularity to scrape
</commit_message>
<xml_diff>
--- a/static/data/top2017_clean.xlsx
+++ b/static/data/top2017_clean.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R101"/>
+  <dimension ref="A1:S101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,11 @@
           <t>genre</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>popularity</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -521,6 +526,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S2" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -585,6 +593,9 @@
           <t>latin</t>
         </is>
       </c>
+      <c r="S3" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -649,6 +660,9 @@
           <t>latin</t>
         </is>
       </c>
+      <c r="S4" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -713,6 +727,9 @@
           <t>tropical house</t>
         </is>
       </c>
+      <c r="S5" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -777,6 +794,9 @@
           <t>trap</t>
         </is>
       </c>
+      <c r="S6" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -841,6 +861,9 @@
           <t>hip hop</t>
         </is>
       </c>
+      <c r="S7" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -905,6 +928,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S8" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -969,6 +995,9 @@
           <t>trap</t>
         </is>
       </c>
+      <c r="S9" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1033,6 +1062,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S10" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1097,6 +1129,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S11" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1161,6 +1196,9 @@
           <t>trap</t>
         </is>
       </c>
+      <c r="S12" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1225,6 +1263,9 @@
           <t>tropical house</t>
         </is>
       </c>
+      <c r="S13" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1289,6 +1330,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S14" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1353,6 +1397,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S15" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1417,6 +1464,9 @@
           <t>trap</t>
         </is>
       </c>
+      <c r="S16" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1481,6 +1531,9 @@
           <t>rap</t>
         </is>
       </c>
+      <c r="S17" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1545,6 +1598,9 @@
           <t>pop rap</t>
         </is>
       </c>
+      <c r="S18" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1609,6 +1665,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S19" t="n">
+        <v>79</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1673,6 +1732,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S20" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1737,6 +1799,9 @@
           <t>other</t>
         </is>
       </c>
+      <c r="S21" t="n">
+        <v>89</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1801,6 +1866,9 @@
           <t>reggaeton</t>
         </is>
       </c>
+      <c r="S22" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1865,6 +1933,9 @@
           <t>other</t>
         </is>
       </c>
+      <c r="S23" t="n">
+        <v>86</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1929,6 +2000,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S24" t="n">
+        <v>86</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1993,6 +2067,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S25" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2057,6 +2134,9 @@
           <t>reggaeton</t>
         </is>
       </c>
+      <c r="S26" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2121,6 +2201,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S27" t="n">
+        <v>72</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2185,6 +2268,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S28" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2249,6 +2335,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S29" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2313,6 +2402,9 @@
           <t>tropical house</t>
         </is>
       </c>
+      <c r="S30" t="n">
+        <v>86</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2377,6 +2469,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S31" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2441,6 +2536,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S32" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2505,6 +2603,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S33" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2569,6 +2670,9 @@
           <t>trap</t>
         </is>
       </c>
+      <c r="S34" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2633,6 +2737,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S35" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2697,6 +2804,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S36" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2761,6 +2871,9 @@
           <t>hip hop</t>
         </is>
       </c>
+      <c r="S37" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2825,6 +2938,9 @@
           <t>hip hop</t>
         </is>
       </c>
+      <c r="S38" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2889,6 +3005,9 @@
           <t>rap</t>
         </is>
       </c>
+      <c r="S39" t="n">
+        <v>89</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2953,6 +3072,9 @@
           <t>tropical house</t>
         </is>
       </c>
+      <c r="S40" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3017,6 +3139,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3081,6 +3206,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S42" t="n">
+        <v>89</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3145,6 +3273,9 @@
           <t>other</t>
         </is>
       </c>
+      <c r="S43" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3209,6 +3340,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S44" t="n">
+        <v>72</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3273,6 +3407,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S45" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3337,6 +3474,9 @@
           <t>reggaeton</t>
         </is>
       </c>
+      <c r="S46" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3401,6 +3541,9 @@
           <t>pop rap</t>
         </is>
       </c>
+      <c r="S47" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3465,6 +3608,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S48" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3529,6 +3675,9 @@
           <t>latin</t>
         </is>
       </c>
+      <c r="S49" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3593,6 +3742,9 @@
           <t>trap</t>
         </is>
       </c>
+      <c r="S50" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3657,6 +3809,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S51" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3721,6 +3876,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S52" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3785,6 +3943,9 @@
           <t>hip hop</t>
         </is>
       </c>
+      <c r="S53" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3849,6 +4010,9 @@
           <t>other</t>
         </is>
       </c>
+      <c r="S54" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3913,6 +4077,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S55" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3977,6 +4144,9 @@
           <t>hip hop</t>
         </is>
       </c>
+      <c r="S56" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4041,6 +4211,9 @@
           <t>latin</t>
         </is>
       </c>
+      <c r="S57" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4105,6 +4278,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S58" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4169,6 +4345,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S59" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -4233,6 +4412,9 @@
           <t>hip hop</t>
         </is>
       </c>
+      <c r="S60" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -4297,6 +4479,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S61" t="n">
+        <v>79</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -4361,6 +4546,9 @@
           <t>hip hop</t>
         </is>
       </c>
+      <c r="S62" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4425,6 +4613,9 @@
           <t>reggaeton</t>
         </is>
       </c>
+      <c r="S63" t="n">
+        <v>72</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4489,6 +4680,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S64" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4553,6 +4747,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S65" t="n">
+        <v>72</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4617,6 +4814,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S66" t="n">
+        <v>67</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4681,6 +4881,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S67" t="n">
+        <v>67</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -4745,6 +4948,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S68" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -4809,6 +5015,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S69" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -4873,6 +5082,9 @@
           <t>reggaeton</t>
         </is>
       </c>
+      <c r="S70" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -4937,6 +5149,9 @@
           <t>trap</t>
         </is>
       </c>
+      <c r="S71" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -5001,6 +5216,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S72" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -5065,6 +5283,9 @@
           <t>rap</t>
         </is>
       </c>
+      <c r="S73" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -5129,6 +5350,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S74" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -5193,6 +5417,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S75" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -5257,6 +5484,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S76" t="n">
+        <v>66</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -5321,6 +5551,9 @@
           <t>other</t>
         </is>
       </c>
+      <c r="S77" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -5385,6 +5618,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S78" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -5449,6 +5685,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S79" t="n">
+        <v>62</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -5513,6 +5752,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S80" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -5577,6 +5819,9 @@
           <t>pop rap</t>
         </is>
       </c>
+      <c r="S81" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -5641,6 +5886,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S82" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -5705,6 +5953,9 @@
           <t>reggaeton</t>
         </is>
       </c>
+      <c r="S83" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -5769,6 +6020,9 @@
           <t>pop rap</t>
         </is>
       </c>
+      <c r="S84" t="n">
+        <v>71</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -5833,6 +6087,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S85" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -5897,6 +6154,9 @@
           <t>reggaeton</t>
         </is>
       </c>
+      <c r="S86" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -5961,6 +6221,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S87" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -6025,6 +6288,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S88" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -6089,6 +6355,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S89" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -6153,6 +6422,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S90" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -6217,6 +6489,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S91" t="n">
+        <v>88</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -6281,6 +6556,9 @@
           <t>other</t>
         </is>
       </c>
+      <c r="S92" t="n">
+        <v>62</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -6345,6 +6623,9 @@
           <t>edm</t>
         </is>
       </c>
+      <c r="S93" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -6409,6 +6690,9 @@
           <t>reggaeton</t>
         </is>
       </c>
+      <c r="S94" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -6473,6 +6757,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S95" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -6537,6 +6824,9 @@
           <t>trap</t>
         </is>
       </c>
+      <c r="S96" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -6601,6 +6891,9 @@
           <t>pop rap</t>
         </is>
       </c>
+      <c r="S97" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -6665,6 +6958,9 @@
           <t>tropical house</t>
         </is>
       </c>
+      <c r="S98" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -6729,6 +7025,9 @@
           <t>other</t>
         </is>
       </c>
+      <c r="S99" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -6793,6 +7092,9 @@
           <t>pop</t>
         </is>
       </c>
+      <c r="S100" t="n">
+        <v>72</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -6856,6 +7158,9 @@
         <is>
           <t>pop</t>
         </is>
+      </c>
+      <c r="S101" t="n">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed scrape to have correct titles
</commit_message>
<xml_diff>
--- a/static/data/top2017_clean.xlsx
+++ b/static/data/top2017_clean.xlsx
@@ -739,7 +739,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>I'm the One</t>
+          <t>I'm Not The Only One</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -873,7 +873,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>It Ain't Me (with Selena Gomez)</t>
+          <t>It Ain’t Me (with Selena Gomez)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>XO TOUR Llif3</t>
+          <t>XO Tour Llif3</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>Ni**as In Paris</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Wild Thoughts</t>
+          <t>Wild Thoughts (feat. Rihanna &amp; Bryson Tiller)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2950,7 +2950,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>rockstar</t>
+          <t>rockstar (feat. 21 Savage)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -3084,7 +3084,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2U (feat. Justin Bieber)</t>
+          <t>2U (Originally Performed by David Guetta Feat. Justin Bieber) - Karaoke Version</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Perfect</t>
+          <t>Ballin' (with Roddy Ricch)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Feels</t>
+          <t>Feels Like Summer</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -3352,7 +3352,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Mama</t>
+          <t>Mama Cry</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -3620,7 +3620,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Chantaje</t>
+          <t>Chantaje (feat. Maluma)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3754,7 +3754,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Havana</t>
+          <t>Havana (feat. Young Thug)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -4625,7 +4625,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>You Don't Know Me - Radio Edit</t>
+          <t>You Don't Know Me (feat. Duane Harden) - Radio Edit</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -4893,7 +4893,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>How Far I'll Go - From "Moana"</t>
+          <t>How Far I'll Go (From "Moana")</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -6032,7 +6032,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Side To Side</t>
+          <t>side to side - live</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -6099,7 +6099,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Otra Vez (feat. J Balvin)</t>
+          <t>Otra vez (feat. J Balvin)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -6367,7 +6367,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Malibu</t>
+          <t>Malibu Nights</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -6434,7 +6434,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>All Night</t>
+          <t>Up All Night</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -6501,7 +6501,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Hear Me Now</t>
+          <t>Hear Me Now (feat. DIAMANTE)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -6702,7 +6702,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Friends (with BloodPop¨)</t>
+          <t>Friends (with BloodPop®)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">

</xml_diff>